<commit_message>
further updates of the code
</commit_message>
<xml_diff>
--- a/technology_technical_economic_parameters.xlsx
+++ b/technology_technical_economic_parameters.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/caneta_cardiff_ac_uk/Documents/04 - Projects/18 - ABM/01 - Code/ABM code - Dec 2021/Code_WH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="701" documentId="11_EC9B91DDB8EEBBF87EB0692D678B75A84151B5BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE8D5886-14D3-4DB4-BFAB-847E45B1426B}"/>
+  <xr:revisionPtr revIDLastSave="822" documentId="11_EC9B91DDB8EEBBF87EB0692D678B75A84151B5BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D515AD47-C8BC-4C57-BC52-23EDF84432AF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7545" yWindow="8730" windowWidth="21600" windowHeight="9015" tabRatio="464" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3705" yWindow="7020" windowWidth="21600" windowHeight="9015" tabRatio="464" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="economic_parameters" sheetId="10" r:id="rId1"/>
     <sheet name="technical_parameters" sheetId="16" r:id="rId2"/>
-    <sheet name="Peak_demand_data" sheetId="15" state="hidden" r:id="rId3"/>
-    <sheet name="workbook_parameters" sheetId="3" r:id="rId4"/>
-    <sheet name="Technology" sheetId="1" state="hidden" r:id="rId5"/>
+    <sheet name="Bus constraints" sheetId="17" r:id="rId3"/>
+    <sheet name="Peak_demand_data" sheetId="15" state="hidden" r:id="rId4"/>
+    <sheet name="workbook_parameters" sheetId="3" r:id="rId5"/>
+    <sheet name="Technology" sheetId="1" state="hidden" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="cop_large_hp">workbook_parameters!#REF!</definedName>
@@ -61,7 +62,7 @@
     <author>tc={AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}</author>
   </authors>
   <commentList>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="95">
   <si>
     <t>Scale</t>
   </si>
@@ -268,9 +269,6 @@
     <t>Renewable_Flag</t>
   </si>
   <si>
-    <t>CFD_Flag</t>
-  </si>
-  <si>
     <t>Capacity_Market_Flag</t>
   </si>
   <si>
@@ -331,12 +329,6 @@
     <t>Capacity_Factor</t>
   </si>
   <si>
-    <t>GBMaxBuildRate</t>
-  </si>
-  <si>
-    <t>MaxBuildRate</t>
-  </si>
-  <si>
     <t>GHG_Emissions_kgCO2/kWh</t>
   </si>
   <si>
@@ -356,6 +348,21 @@
   </si>
   <si>
     <t>Hydro/2018_GB_Hydro_MW.txt</t>
+  </si>
+  <si>
+    <t>GBMaxBuildRate_kW</t>
+  </si>
+  <si>
+    <t>Busbars</t>
+  </si>
+  <si>
+    <t>CfD_eligible</t>
+  </si>
+  <si>
+    <t>CfD_Flag</t>
+  </si>
+  <si>
+    <t>Typical_Capacity_kW</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1026,10 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1411,7 +1418,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="M1" dT="2022-01-12T12:32:53.44" personId="{180F677F-290E-46C7-A175-9F51A1040FF7}" id="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
+  <threadedComment ref="N1" dT="2022-01-12T12:32:53.44" personId="{180F677F-290E-46C7-A175-9F51A1040FF7}" id="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
     <text>(used as a key to get the wholesale price of the fuel for each technology)</text>
   </threadedComment>
 </ThreadedComments>
@@ -1424,10 +1431,10 @@
   </sheetPr>
   <dimension ref="A1:BC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="C4" sqref="C4"/>
+      <selection pane="topRight" activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1469,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>49</v>
@@ -1602,7 +1609,7 @@
         <v>52</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>44</v>
@@ -1769,7 +1776,7 @@
         <v>52</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>46</v>
@@ -1908,7 +1915,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>47</v>
@@ -2047,7 +2054,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>44</v>
@@ -2186,7 +2193,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>46</v>
@@ -2325,7 +2332,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>47</v>
@@ -2464,7 +2471,7 @@
         <v>59</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>44</v>
@@ -2603,7 +2610,7 @@
         <v>59</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>46</v>
@@ -2742,7 +2749,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>47</v>
@@ -2881,7 +2888,7 @@
         <v>56</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>44</v>
@@ -3020,7 +3027,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>46</v>
@@ -3159,7 +3166,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>47</v>
@@ -3298,7 +3305,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>44</v>
@@ -3437,7 +3444,7 @@
         <v>57</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>46</v>
@@ -3576,7 +3583,7 @@
         <v>57</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>47</v>
@@ -3715,7 +3722,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>44</v>
@@ -3854,7 +3861,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>46</v>
@@ -3993,7 +4000,7 @@
         <v>43</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>47</v>
@@ -4132,7 +4139,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>44</v>
@@ -4271,7 +4278,7 @@
         <v>54</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>46</v>
@@ -4408,7 +4415,7 @@
         <v>54</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>47</v>
@@ -4545,7 +4552,7 @@
         <v>61</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>44</v>
@@ -4682,7 +4689,7 @@
         <v>61</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>46</v>
@@ -4819,7 +4826,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>47</v>
@@ -4956,7 +4963,7 @@
         <v>60</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>44</v>
@@ -5093,7 +5100,7 @@
         <v>60</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>46</v>
@@ -5230,7 +5237,7 @@
         <v>60</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>47</v>
@@ -5367,7 +5374,7 @@
         <v>58</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>44</v>
@@ -5504,7 +5511,7 @@
         <v>58</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>46</v>
@@ -5641,7 +5648,7 @@
         <v>58</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>47</v>
@@ -5778,7 +5785,7 @@
         <v>55</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>44</v>
@@ -5915,7 +5922,7 @@
         <v>55</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>46</v>
@@ -6052,7 +6059,7 @@
         <v>55</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>47</v>
@@ -6186,10 +6193,10 @@
     </row>
     <row r="35" spans="1:55" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>44</v>
@@ -6353,10 +6360,10 @@
     </row>
     <row r="36" spans="1:55" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>46</v>
@@ -6492,10 +6499,10 @@
     </row>
     <row r="37" spans="1:55" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>47</v>
@@ -6638,11 +6645,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B9EF98-BE57-4B2E-A22F-A59E6D68BD28}">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6651,82 +6658,90 @@
     <col min="2" max="3" width="36.5703125" style="8" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
-      </c>
       <c r="N1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" t="s">
         <v>80</v>
-      </c>
-      <c r="O1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" t="s">
-        <v>83</v>
       </c>
       <c r="Q1" t="s">
         <v>82</v>
       </c>
       <c r="R1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="U1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" t="s">
         <v>84</v>
       </c>
-      <c r="S1" t="s">
-        <v>85</v>
-      </c>
-      <c r="T1" t="s">
-        <v>86</v>
-      </c>
-      <c r="U1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="8">
         <v>25</v>
@@ -6747,48 +6762,51 @@
         <v>0</v>
       </c>
       <c r="I2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
         <v>5</v>
       </c>
-      <c r="L2" s="8">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2">
+      <c r="M2" s="8">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2">
         <v>3</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>2</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>0.45300000000000001</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.85</v>
       </c>
-      <c r="R2" s="22">
+      <c r="S2" s="23">
         <v>2000000</v>
       </c>
-      <c r="S2" s="22">
+      <c r="T2" s="23">
         <v>350000</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.36499999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="8">
         <v>25</v>
@@ -6809,48 +6827,51 @@
         <v>0</v>
       </c>
       <c r="I3" s="8">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8">
         <v>3</v>
       </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
       <c r="K3" s="8">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8">
         <v>6</v>
       </c>
-      <c r="L3" s="8">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
       <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
         <v>0.19</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>0.92</v>
       </c>
-      <c r="R3" s="22">
+      <c r="S3" s="23">
         <v>1000000</v>
       </c>
-      <c r="S3" s="22">
+      <c r="T3" s="23">
         <v>500000</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.46</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="8">
         <v>25</v>
@@ -6877,42 +6898,45 @@
         <v>0</v>
       </c>
       <c r="K4" s="8">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
         <v>7</v>
       </c>
-      <c r="L4" s="8">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="M4" s="8">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
         <v>54</v>
-      </c>
-      <c r="N4">
-        <v>6</v>
       </c>
       <c r="O4">
         <v>6</v>
       </c>
       <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
         <v>0.17</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.88</v>
       </c>
-      <c r="R4" s="22">
+      <c r="S4" s="23">
         <v>2000000</v>
       </c>
-      <c r="S4" s="22">
+      <c r="T4" s="23">
         <v>100000</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>0.90700000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="8">
         <v>60</v>
@@ -6924,7 +6948,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -6933,48 +6957,51 @@
         <v>0</v>
       </c>
       <c r="I5" s="8">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8">
         <v>2</v>
       </c>
-      <c r="J5" s="8">
-        <v>1</v>
-      </c>
       <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8">
         <v>2</v>
       </c>
-      <c r="L5" s="8">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>75</v>
-      </c>
-      <c r="N5">
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>74</v>
+      </c>
+      <c r="O5">
         <v>8</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>5</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>0.77400000000000002</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.81</v>
       </c>
-      <c r="R5" s="22">
+      <c r="S5" s="23">
         <v>1000000</v>
       </c>
-      <c r="S5" s="22">
+      <c r="T5" s="23">
         <v>1000000</v>
       </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="8">
         <v>22</v>
@@ -6986,60 +7013,63 @@
         <v>1</v>
       </c>
       <c r="F6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
         <v>8700</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>1341.2</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J6" s="8">
         <v>5</v>
       </c>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
       <c r="K6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="8">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6">
         <v>5</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>3</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.48</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.24</v>
       </c>
-      <c r="R6" s="22">
+      <c r="S6" s="23">
         <v>1000000</v>
       </c>
-      <c r="S6" s="22">
+      <c r="T6" s="23">
         <v>56000</v>
       </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6" s="22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="8">
         <v>24</v>
@@ -7051,60 +7081,63 @@
         <v>0</v>
       </c>
       <c r="F7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
         <v>12100</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>5564</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="8">
         <v>4</v>
       </c>
-      <c r="J7" s="8">
-        <v>1</v>
-      </c>
       <c r="K7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="8">
-        <v>1</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7">
         <v>4</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>2</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0.32</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.17</v>
       </c>
-      <c r="R7" s="22">
+      <c r="S7" s="23">
         <v>550000</v>
       </c>
-      <c r="S7" s="22">
+      <c r="T7" s="23">
         <v>30600</v>
       </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="8">
         <v>25</v>
@@ -7116,60 +7149,63 @@
         <v>0</v>
       </c>
       <c r="F8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
         <v>13000</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>111</v>
       </c>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
       <c r="J8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="8">
-        <v>1</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
         <v>0.11</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>0.12</v>
       </c>
-      <c r="R8" s="22">
+      <c r="S8" s="23">
         <v>1500000</v>
       </c>
-      <c r="S8" s="22">
+      <c r="T8" s="23">
         <v>100000</v>
       </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="8">
         <v>41</v>
@@ -7181,7 +7217,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="8">
         <v>0</v>
@@ -7190,51 +7226,54 @@
         <v>0</v>
       </c>
       <c r="I9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8">
         <v>2</v>
       </c>
-      <c r="J9" s="8">
-        <v>1</v>
-      </c>
       <c r="K9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="8">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>77</v>
-      </c>
-      <c r="N9">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>76</v>
       </c>
       <c r="O9">
         <v>2</v>
       </c>
       <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9">
         <v>0.35</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>0.84</v>
       </c>
-      <c r="R9" s="22">
+      <c r="S9" s="23">
         <v>60000</v>
       </c>
-      <c r="S9" s="22">
+      <c r="T9" s="23">
         <v>10000</v>
       </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="8">
         <v>25</v>
@@ -7255,48 +7294,51 @@
         <v>0</v>
       </c>
       <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="8">
         <v>5</v>
       </c>
-      <c r="J10" s="8">
-        <v>1</v>
-      </c>
       <c r="K10" s="8">
+        <v>1</v>
+      </c>
+      <c r="L10" s="8">
         <v>3</v>
       </c>
-      <c r="L10" s="8">
-        <v>1</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N10">
+      <c r="M10" s="8">
+        <v>1</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10">
         <v>2</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>3</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>0.84</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.88</v>
       </c>
-      <c r="R10" s="22">
+      <c r="S10" s="23">
         <v>500000</v>
       </c>
-      <c r="S10" s="22">
+      <c r="T10" s="23">
         <v>14000</v>
       </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="8">
         <v>25</v>
@@ -7308,7 +7350,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
@@ -7317,48 +7359,51 @@
         <v>0</v>
       </c>
       <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8">
         <v>4</v>
       </c>
-      <c r="J11" s="8">
-        <v>0</v>
-      </c>
       <c r="K11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="8">
         <v>1</v>
       </c>
-      <c r="M11" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="8">
+        <v>1</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O11">
         <v>2</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>3</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>0.45</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0.88</v>
       </c>
-      <c r="R11" s="22">
+      <c r="S11" s="23">
         <v>500000</v>
       </c>
-      <c r="S11" s="22">
+      <c r="T11" s="23">
         <v>500000</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>-0.29499999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="8">
         <v>25</v>
@@ -7370,7 +7415,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
@@ -7379,48 +7424,51 @@
         <v>0</v>
       </c>
       <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8">
         <v>6</v>
       </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
       <c r="K12" s="8">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
         <v>4</v>
       </c>
-      <c r="L12" s="8">
-        <v>1</v>
-      </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="8">
+        <v>1</v>
+      </c>
+      <c r="N12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>3</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>0.45300000000000001</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0.85</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1.5</v>
       </c>
-      <c r="S12">
+      <c r="T12" s="8">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="8">
         <f>C2</f>
@@ -7431,21 +7479,23 @@
         <v>0</v>
       </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M13" s="8"/>
+      <c r="N13" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -7453,6 +7503,7 @@
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7461,6 +7512,1176 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898708BB-497B-47A9-8A42-DFB40CA3BBD6}">
+  <dimension ref="A1:AB31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="31" width="4.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8">
+        <v>1</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8">
+        <v>1</v>
+      </c>
+      <c r="M4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8">
+        <v>1</v>
+      </c>
+      <c r="M6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8">
+        <v>1</v>
+      </c>
+      <c r="M9" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8">
+        <v>1</v>
+      </c>
+      <c r="M10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1</v>
+      </c>
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8">
+        <v>1</v>
+      </c>
+      <c r="M12" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8">
+        <v>1</v>
+      </c>
+      <c r="M13" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8">
+        <v>1</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1</v>
+      </c>
+      <c r="L14" s="8">
+        <v>1</v>
+      </c>
+      <c r="M14" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8">
+        <v>1</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1</v>
+      </c>
+      <c r="L15" s="8">
+        <v>1</v>
+      </c>
+      <c r="M15" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8">
+        <v>1</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>1</v>
+      </c>
+      <c r="M16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8">
+        <v>1</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1</v>
+      </c>
+      <c r="L17" s="8">
+        <v>1</v>
+      </c>
+      <c r="M17" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8">
+        <v>1</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1</v>
+      </c>
+      <c r="L18" s="8">
+        <v>1</v>
+      </c>
+      <c r="M18" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1</v>
+      </c>
+      <c r="L19" s="8">
+        <v>1</v>
+      </c>
+      <c r="M19" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8">
+        <v>1</v>
+      </c>
+      <c r="K20" s="8">
+        <v>1</v>
+      </c>
+      <c r="L20" s="8">
+        <v>1</v>
+      </c>
+      <c r="M20" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+      <c r="G21" s="8">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8">
+        <v>1</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8">
+        <v>1</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1</v>
+      </c>
+      <c r="M21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8">
+        <v>1</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8">
+        <v>1</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8">
+        <v>1</v>
+      </c>
+      <c r="M22" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>1</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8">
+        <v>1</v>
+      </c>
+      <c r="H23" s="8">
+        <v>1</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8">
+        <v>1</v>
+      </c>
+      <c r="K23" s="8">
+        <v>1</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1</v>
+      </c>
+      <c r="M23" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8">
+        <v>1</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8">
+        <v>1</v>
+      </c>
+      <c r="K24" s="8">
+        <v>1</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1</v>
+      </c>
+      <c r="M24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="8">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8">
+        <v>1</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1</v>
+      </c>
+      <c r="L25" s="8">
+        <v>1</v>
+      </c>
+      <c r="M25" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8">
+        <v>1</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8">
+        <v>1</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8">
+        <v>1</v>
+      </c>
+      <c r="M26" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8">
+        <v>1</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8">
+        <v>1</v>
+      </c>
+      <c r="K27" s="8">
+        <v>1</v>
+      </c>
+      <c r="L27" s="8">
+        <v>1</v>
+      </c>
+      <c r="M27" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
+      </c>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8">
+        <v>1</v>
+      </c>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8">
+        <v>1</v>
+      </c>
+      <c r="M28" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8">
+        <v>1</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8">
+        <v>1</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1</v>
+      </c>
+      <c r="L29" s="8">
+        <v>1</v>
+      </c>
+      <c r="M29" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8">
+        <v>1</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8">
+        <v>1</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8">
+        <v>1</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8">
+        <v>1</v>
+      </c>
+      <c r="M30" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8">
+        <v>1</v>
+      </c>
+      <c r="G31" s="8">
+        <v>1</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1</v>
+      </c>
+      <c r="I31" s="8">
+        <v>1</v>
+      </c>
+      <c r="J31" s="8">
+        <v>1</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1</v>
+      </c>
+      <c r="L31" s="8">
+        <v>1</v>
+      </c>
+      <c r="M31" s="8">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -7529,7 +8750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
@@ -7559,7 +8780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:P21"/>
   <sheetViews>
@@ -7897,6 +9118,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000F5CD42354AAC441BBEBC0DB60FF2E5E" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ea4030731fbb82b60f08fc005274800f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="77004af6-74ae-4ef6-bd6c-a07f36984bb1" xmlns:ns3="fc548c4c-0127-4895-9309-6e27078b8b5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="14d4a3203feaba80961c8c11a30ae70b" ns2:_="" ns3:_="">
     <xsd:import namespace="77004af6-74ae-4ef6-bd6c-a07f36984bb1"/>
@@ -8101,15 +9331,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C816199B-3615-49AE-8787-402FADC64DE2}">
   <ds:schemaRefs>
@@ -8120,6 +9341,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE276612-2441-44A6-B645-D8B674E952AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A2448F5-A512-4284-A3B0-EE93AC3A811B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8138,14 +9367,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE276612-2441-44A6-B645-D8B674E952AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{bdb74b30-9568-4856-bdbf-06759778fcbc}" enabled="0" method="" siteId="{bdb74b30-9568-4856-bdbf-06759778fcbc}" removed="1"/>

</xml_diff>

<commit_message>
creation of the ABM class
</commit_message>
<xml_diff>
--- a/technology_technical_economic_parameters.xlsx
+++ b/technology_technical_economic_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cf-my.sharepoint.com/personal/caneta_cardiff_ac_uk/Documents/04 - Projects/18 - ABM/01 - Code/ABM code - Dec 2021/Code_WH/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="916" documentId="11_EC9B91DDB8EEBBF87EB0692D678B75A84151B5BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AEECC79-1A5F-4D7A-9F5C-9DBF93D3E6F4}"/>
+  <xr:revisionPtr revIDLastSave="957" documentId="11_EC9B91DDB8EEBBF87EB0692D678B75A84151B5BA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AC06E29-C201-4FD6-87BE-2605A53D08C8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="464" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="464" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="economic_parameters" sheetId="10" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <author>tc={AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="99">
   <si>
     <t>Scale</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t>Capacity_Market_eligible</t>
+  </si>
+  <si>
+    <t>Expected_Market_Ready_Time</t>
+  </si>
+  <si>
+    <t>Li-Battery</t>
+  </si>
+  <si>
+    <t>Storage_Flag</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1421,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="N1" dT="2022-01-12T12:32:53.44" personId="{180F677F-290E-46C7-A175-9F51A1040FF7}" id="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
+  <threadedComment ref="O1" dT="2022-01-12T12:32:53.44" personId="{180F677F-290E-46C7-A175-9F51A1040FF7}" id="{AF8E16E6-1772-48C9-B6C8-8ED2AAF161CC}">
     <text>(used as a key to get the wholesale price of the fuel for each technology)</text>
   </threadedComment>
 </ThreadedComments>
@@ -1428,7 +1437,7 @@
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="topRight" activeCell="F43" sqref="F43"/>
+      <selection pane="topRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1459,7 @@
     <col min="24" max="24" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="97.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="31" max="44" width="10" bestFit="1" customWidth="1"/>
@@ -5806,52 +5815,52 @@
         <v>45</v>
       </c>
       <c r="E23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="F23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="G23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="H23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="I23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="J23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="K23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="L23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="M23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="N23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="O23" s="16">
-        <v>535148.53691693849</v>
+        <v>539112.5</v>
       </c>
       <c r="P23" s="16">
-        <v>531980.00713934947</v>
+        <v>539112.5</v>
       </c>
       <c r="Q23" s="16">
-        <v>520466.09476176166</v>
+        <v>539112.5</v>
       </c>
       <c r="R23" s="16">
-        <v>525641.36076692073</v>
+        <v>539112.5</v>
       </c>
       <c r="S23" s="16">
-        <v>530841.53251300007</v>
+        <v>539112.5</v>
       </c>
       <c r="T23" s="16">
-        <v>536066.69499999995</v>
+        <v>539112.5</v>
       </c>
       <c r="U23" s="16">
         <v>539112.5</v>
@@ -6397,55 +6406,55 @@
         <v>45</v>
       </c>
       <c r="E26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="F26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="G26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="H26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="I26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="J26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="K26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="L26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="M26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="N26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="O26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="P26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="Q26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="R26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="S26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="T26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="U26" s="16">
-        <v>0</v>
+        <v>3396599.9999999995</v>
       </c>
       <c r="V26" s="16">
         <v>3396599.9999999995</v>
@@ -8756,33 +8765,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B9EF98-BE57-4B2E-A22F-A59E6D68BD28}">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F23" sqref="F23"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="36.5703125" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="36.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.140625" customWidth="1"/>
+    <col min="24" max="24" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>51</v>
       </c>
@@ -8793,67 +8802,73 @@
         <v>77</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>84</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>78</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>81</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>80</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>82</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>83</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>94</v>
       </c>
+      <c r="Y1" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>52</v>
       </c>
@@ -8873,56 +8888,62 @@
         <v>0</v>
       </c>
       <c r="G2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="8">
         <v>0</v>
       </c>
       <c r="J2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8">
         <v>5</v>
       </c>
-      <c r="M2" s="8">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N2" s="8">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
         <v>74</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>3</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>2</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0.45300000000000001</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>0.85</v>
       </c>
-      <c r="S2" s="20">
-        <f>W2</f>
+      <c r="T2" s="20">
+        <f>X2</f>
         <v>2000000</v>
       </c>
-      <c r="T2" s="19">
+      <c r="U2" s="19">
         <v>250000</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>0.36499999999999999</v>
       </c>
-      <c r="W2" s="19">
+      <c r="X2" s="19">
         <v>2000000</v>
       </c>
+      <c r="Y2">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>53</v>
       </c>
@@ -8942,56 +8963,62 @@
         <v>0</v>
       </c>
       <c r="G3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="8">
         <v>0</v>
       </c>
       <c r="J3" s="8">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
         <v>3</v>
       </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
       <c r="L3" s="8">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8">
         <v>6</v>
       </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="8">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
       <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
         <v>0.19</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>0.92</v>
       </c>
-      <c r="S3" s="20">
-        <f t="shared" ref="S3:S13" si="0">W3</f>
+      <c r="T3" s="20">
+        <f t="shared" ref="T3:T13" si="0">X3</f>
         <v>1000000</v>
       </c>
-      <c r="T3" s="19">
+      <c r="U3" s="19">
         <v>500000</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>0.46</v>
       </c>
-      <c r="W3" s="19">
+      <c r="X3" s="19">
         <v>1000000</v>
       </c>
+      <c r="Y3" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>54</v>
       </c>
@@ -9011,10 +9038,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="8">
         <v>0</v>
@@ -9026,41 +9053,47 @@
         <v>0</v>
       </c>
       <c r="L4" s="8">
+        <v>0</v>
+      </c>
+      <c r="M4" s="8">
         <v>7</v>
       </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="N4" s="8">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>54</v>
-      </c>
-      <c r="O4">
-        <v>6</v>
       </c>
       <c r="P4">
         <v>6</v>
       </c>
       <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="R4">
         <v>0.17</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.88</v>
       </c>
-      <c r="S4" s="20">
+      <c r="T4" s="20">
         <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
-      <c r="T4" s="19">
+      <c r="U4" s="19">
         <v>100000</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.90700000000000003</v>
       </c>
-      <c r="W4" s="19">
+      <c r="X4" s="19">
         <v>2000000</v>
       </c>
+      <c r="Y4" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>55</v>
       </c>
@@ -9077,59 +9110,65 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
       </c>
       <c r="H5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="8">
         <v>0</v>
       </c>
       <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
         <v>2</v>
       </c>
-      <c r="K5" s="8">
-        <v>1</v>
-      </c>
       <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
         <v>2</v>
       </c>
-      <c r="M5" s="8">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
         <v>73</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>8</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>5</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.77400000000000002</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.81</v>
       </c>
-      <c r="S5" s="20">
+      <c r="T5" s="20">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="T5" s="19">
+      <c r="U5" s="19">
         <v>1000000</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="W5" s="19">
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="X5" s="19">
         <v>1000000</v>
       </c>
+      <c r="Y5" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>56</v>
       </c>
@@ -9140,7 +9179,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="8">
         <v>1</v>
@@ -9149,59 +9188,65 @@
         <v>1</v>
       </c>
       <c r="G6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
         <v>8700</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J6" s="8">
         <v>1341.2</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>5</v>
       </c>
-      <c r="K6" s="8">
-        <v>1</v>
-      </c>
       <c r="L6" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="8">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
         <v>75</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>5</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>3</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.48</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.24</v>
       </c>
-      <c r="S6" s="20">
+      <c r="T6" s="20">
         <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
-      <c r="T6" s="19">
+      <c r="U6" s="19">
         <v>50000</v>
       </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6" s="18" t="s">
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="W6" s="19">
+      <c r="X6" s="19">
         <v>1000000</v>
       </c>
+      <c r="Y6" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>57</v>
       </c>
@@ -9212,68 +9257,74 @@
         <v>24</v>
       </c>
       <c r="D7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8">
         <v>12100</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J7" s="8">
         <v>5564</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>4</v>
       </c>
-      <c r="K7" s="8">
-        <v>1</v>
-      </c>
       <c r="L7" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="8">
-        <v>1</v>
-      </c>
-      <c r="N7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="8">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>4</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>2</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.32</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>0.17</v>
       </c>
-      <c r="S7" s="20">
+      <c r="T7" s="20">
         <f t="shared" si="0"/>
         <v>550000</v>
       </c>
-      <c r="T7" s="19">
+      <c r="U7" s="19">
         <v>30000</v>
       </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7" s="17" t="s">
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="W7" s="19">
+      <c r="X7" s="19">
         <v>550000</v>
       </c>
+      <c r="Y7" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>43</v>
       </c>
@@ -9284,68 +9335,75 @@
         <v>25</v>
       </c>
       <c r="D8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
         <v>13000</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J8" s="8">
         <v>111</v>
       </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
       <c r="K8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="8">
-        <v>1</v>
-      </c>
-      <c r="N8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
       <c r="P8">
         <v>1</v>
       </c>
       <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
         <v>0.11</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8" s="20">
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" s="20">
         <f t="shared" si="0"/>
         <v>1500000</v>
       </c>
-      <c r="T8" s="19">
-        <v>100000</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8" s="17" t="s">
+      <c r="U8" s="19">
+        <f>(I8-J8)/8*1000/2</f>
+        <v>805562.5</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="W8" s="19">
+      <c r="X8" s="19">
         <v>1500000</v>
       </c>
+      <c r="Y8" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -9356,16 +9414,16 @@
         <v>41</v>
       </c>
       <c r="D9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
@@ -9374,50 +9432,56 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8">
         <v>2</v>
       </c>
-      <c r="K9" s="8">
-        <v>1</v>
-      </c>
       <c r="L9" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="8">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="8">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
         <v>75</v>
-      </c>
-      <c r="O9">
-        <v>2</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
       <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
         <v>0.35</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>0.84</v>
       </c>
-      <c r="S9" s="20">
+      <c r="T9" s="20">
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-      <c r="T9" s="19">
+      <c r="U9" s="19">
         <v>10000</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9" s="17" t="s">
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="W9" s="19">
+      <c r="X9" s="19">
         <v>60000</v>
       </c>
+      <c r="Y9" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
@@ -9437,56 +9501,62 @@
         <v>0</v>
       </c>
       <c r="G10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="8">
         <v>0</v>
       </c>
       <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
         <v>5</v>
       </c>
-      <c r="K10" s="8">
-        <v>1</v>
-      </c>
       <c r="L10" s="8">
+        <v>1</v>
+      </c>
+      <c r="M10" s="8">
         <v>3</v>
       </c>
-      <c r="M10" s="8">
-        <v>1</v>
-      </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" s="8">
+        <v>1</v>
+      </c>
+      <c r="O10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>2</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>3</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>0.84</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>0.88</v>
       </c>
-      <c r="S10" s="20">
+      <c r="T10" s="20">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="T10" s="19">
+      <c r="U10" s="19">
         <v>14000</v>
       </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="W10" s="19">
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="X10" s="19">
         <v>500000</v>
       </c>
+      <c r="Y10" s="8">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>60</v>
       </c>
@@ -9503,59 +9573,65 @@
         <v>0</v>
       </c>
       <c r="F11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
       </c>
       <c r="H11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="8">
         <v>0</v>
       </c>
       <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8">
         <v>4</v>
       </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
       <c r="L11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="8">
         <v>1</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="8">
+        <v>1</v>
+      </c>
+      <c r="O11" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>2</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>3</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0.45</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>0.88</v>
       </c>
-      <c r="S11" s="20">
+      <c r="T11" s="20">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="T11" s="19">
+      <c r="U11" s="19">
         <v>500000</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>-0.29499999999999998</v>
       </c>
-      <c r="W11" s="19">
+      <c r="X11" s="19">
         <v>500000</v>
       </c>
+      <c r="Y11" s="8">
+        <v>2018</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>61</v>
       </c>
@@ -9572,59 +9648,65 @@
         <v>0</v>
       </c>
       <c r="F12" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="8">
         <v>1</v>
       </c>
       <c r="H12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="8">
         <v>0</v>
       </c>
       <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
         <v>6</v>
       </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
       <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8">
         <v>4</v>
       </c>
-      <c r="M12" s="8">
-        <v>1</v>
-      </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="8">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>3</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>2</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0.45300000000000001</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>0.85</v>
       </c>
-      <c r="S12" s="20">
+      <c r="T12" s="20">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="T12" s="19">
+      <c r="U12" s="19">
         <v>500000</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="W12" s="19">
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="X12" s="19">
         <v>500000</v>
       </c>
+      <c r="Y12" s="8">
+        <v>2035</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>69</v>
       </c>
@@ -9636,40 +9718,54 @@
         <v>25</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" ref="D13" si="1">D2</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" ref="E13" si="1">E2</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="8">
         <v>1</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="8"/>
+      <c r="O13" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="S13" s="20">
+      <c r="T13" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="H14" s="8"/>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10852,7 +10948,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10959,9 +11055,6 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -10970,9 +11063,6 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="F7">
-        <v>1</v>
-      </c>
       <c r="G7">
         <v>1</v>
       </c>
@@ -11127,7 +11217,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>